<commit_message>
my computer is freezing a bit. Committing in order to back up!
</commit_message>
<xml_diff>
--- a/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice.xlsx
+++ b/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Public Opinion on Charter Schools</t>
   </si>
@@ -98,6 +98,45 @@
   <si>
     <t>This excel spreadsheet was generated by manually entering (and visualizing) data from https://www.educationnext.org/files/2018ednextpoll.pdf and from https://educationnext.org/files/ednext-poll-question-wording-over-time-through-2018.pdf</t>
   </si>
+  <si>
+    <t>Charters</t>
+  </si>
+  <si>
+    <t>Vouchers</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Strongly Support</t>
+  </si>
+  <si>
+    <t>Somewhat Support</t>
+  </si>
+  <si>
+    <t>Somewhat Oppose</t>
+  </si>
+  <si>
+    <t>Strongly Oppose</t>
+  </si>
+  <si>
+    <t>Neither Support Nor Oppose</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
 </sst>
 </file>
 
@@ -120,15 +159,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -227,11 +272,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -270,6 +384,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6486,15 +6611,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>175742</xdr:rowOff>
+      <xdr:colOff>10705</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>87206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>173361</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>23203</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>629836</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>116096</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6511,8 +6636,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2187422"/>
-          <a:ext cx="5934081" cy="1859141"/>
+          <a:off x="10705" y="8795777"/>
+          <a:ext cx="5930452" cy="1843176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>58963</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44591</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>179796</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>108368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698499" y="2766020"/>
+          <a:ext cx="10190118" cy="2785205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7667,25 +7830,276 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="22.578125" customWidth="1"/>
+    <col min="4" max="4" width="16.3671875" customWidth="1"/>
+    <col min="5" max="5" width="16.7890625" customWidth="1"/>
+    <col min="6" max="6" width="15.89453125" customWidth="1"/>
+    <col min="7" max="7" width="23.3125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="5" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="25">
+        <v>15</v>
+      </c>
+      <c r="D6" s="25">
+        <v>29</v>
+      </c>
+      <c r="E6" s="25">
+        <v>21</v>
+      </c>
+      <c r="F6" s="25">
+        <v>14</v>
+      </c>
+      <c r="G6" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="23">
+        <v>14</v>
+      </c>
+      <c r="D7" s="23">
+        <v>30</v>
+      </c>
+      <c r="E7" s="23">
+        <v>21</v>
+      </c>
+      <c r="F7" s="23">
+        <v>23</v>
+      </c>
+      <c r="G7" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="25">
+        <v>14</v>
+      </c>
+      <c r="D8" s="25">
+        <v>32</v>
+      </c>
+      <c r="E8" s="25">
+        <v>17</v>
+      </c>
+      <c r="F8" s="25">
+        <v>9</v>
+      </c>
+      <c r="G8" s="26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="23">
+        <v>25</v>
+      </c>
+      <c r="D9" s="23">
+        <v>31</v>
+      </c>
+      <c r="E9" s="23">
+        <v>12</v>
+      </c>
+      <c r="F9" s="23">
+        <v>11</v>
+      </c>
+      <c r="G9" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="25">
+        <v>12</v>
+      </c>
+      <c r="D10" s="25">
+        <v>37</v>
+      </c>
+      <c r="E10" s="25">
+        <v>22</v>
+      </c>
+      <c r="F10" s="25">
+        <v>11</v>
+      </c>
+      <c r="G10" s="26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="23">
+        <v>26</v>
+      </c>
+      <c r="D11" s="23">
+        <v>35</v>
+      </c>
+      <c r="E11" s="23">
+        <v>17</v>
+      </c>
+      <c r="F11" s="23">
+        <v>12</v>
+      </c>
+      <c r="G11" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="25">
+        <v>15</v>
+      </c>
+      <c r="D12" s="25">
+        <v>28</v>
+      </c>
+      <c r="E12" s="25">
+        <v>23</v>
+      </c>
+      <c r="F12" s="25">
+        <v>15</v>
+      </c>
+      <c r="G12" s="26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="23">
+        <v>9</v>
+      </c>
+      <c r="D13" s="23">
+        <v>29</v>
+      </c>
+      <c r="E13" s="23">
+        <v>25</v>
+      </c>
+      <c r="F13" s="23">
+        <v>27</v>
+      </c>
+      <c r="G13" s="24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="20">
+        <v>6</v>
+      </c>
+      <c r="D14" s="20">
+        <v>27</v>
+      </c>
+      <c r="E14" s="20">
+        <v>24</v>
+      </c>
+      <c r="F14" s="20">
+        <v>31</v>
+      </c>
+      <c r="G14" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="23">
+        <v>4</v>
+      </c>
+      <c r="D15" s="23">
+        <v>15</v>
+      </c>
+      <c r="E15" s="23">
+        <v>22</v>
+      </c>
+      <c r="F15" s="23">
+        <v>48</v>
+      </c>
+      <c r="G15" s="24">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>